<commit_message>
-Changed set functions for width and height so that they return a boolean based on whether the set was successful. -Updated the UML diagram to reflect this change.
</commit_message>
<xml_diff>
--- a/Homework 4 UML Diagrams.xlsx
+++ b/Homework 4 UML Diagrams.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin\Google Drive\Whitworth Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin\Source\Repos\CS-172-Homework-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -77,13 +77,13 @@
     <t xml:space="preserve"> +getWidth(): double const</t>
   </si>
   <si>
-    <t xml:space="preserve"> +setWidth(width: double): void</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +getHeight(): double const</t>
   </si>
   <si>
-    <t xml:space="preserve"> +setHeight(height: double): void</t>
+    <t xml:space="preserve"> +setWidth(width: double): bool</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +setHeight(height: double): bool</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="B1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -607,12 +607,12 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B19" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B20" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">

</xml_diff>